<commit_message>
v0.8.1 - showing indicators on output tab
</commit_message>
<xml_diff>
--- a/data/excel/20180926 Regional game IMS 2.4.xlsx
+++ b/data/excel/20180926 Regional game IMS 2.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Raphael\GitProjects\PlanningTool\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5B215F-2B6C-44EB-9B9F-532D4A0C2E49}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8990088-C704-4B0E-A928-DE726575A389}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7980" tabRatio="762" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7980" tabRatio="762" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASIS - Financial data" sheetId="21" r:id="rId1"/>
@@ -3096,7 +3096,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3173,7 +3173,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3227,10 +3226,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3241,6 +3240,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -4073,7 +4074,7 @@
         <f t="shared" ref="D4:D8" si="0">B4-C4</f>
         <v>-656.5318759557772</v>
       </c>
-      <c r="E4" s="65">
+      <c r="E4" s="64">
         <f>SUM('INPUT - Housing per plan '!N3:O3)+SUM('INPUT - Housing per plan '!N19:O21)-'BASIS - Housing demand'!I3</f>
         <v>-806.5318759557772</v>
       </c>
@@ -4115,7 +4116,7 @@
         <f t="shared" si="0"/>
         <v>4980.0822281832079</v>
       </c>
-      <c r="E6" s="65">
+      <c r="E6" s="64">
         <f>SUM('INPUT - Housing per plan '!N11:O18)-'BASIS - Housing demand'!I6</f>
         <v>-2275.1677718167921</v>
       </c>
@@ -4126,7 +4127,7 @@
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="61">
+      <c r="E7" s="60">
         <f>SUM('INPUT - Housing per plan '!N3:O21)-'BASIS - Housing demand'!I7</f>
         <v>-60912.374050490107</v>
       </c>
@@ -4147,7 +4148,7 @@
         <f t="shared" si="0"/>
         <v>4770.9382787234572</v>
       </c>
-      <c r="E8" s="65">
+      <c r="E8" s="64">
         <f>SUM('INPUT - Housing per plan '!N3:O21)-'BASIS - Housing demand'!I8</f>
         <v>-5738.5617212765428</v>
       </c>
@@ -4255,7 +4256,7 @@
       <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="58">
+      <c r="C4" s="57">
         <f>'INPUT - Housing per plan '!T3+SUM('INPUT - Housing per plan '!T19:T21)</f>
         <v>10208915.358117528</v>
       </c>
@@ -4295,7 +4296,7 @@
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="58">
+      <c r="C6" s="57">
         <f>SUM('INPUT - Housing per plan '!T11:T18)</f>
         <v>50312674.829398632</v>
       </c>
@@ -4430,7 +4431,7 @@
       <c r="A25" t="s">
         <v>321</v>
       </c>
-      <c r="B25" s="58">
+      <c r="B25" s="57">
         <f>'INPUT - Housing per plan '!T11+'INPUT - Housing per plan '!T12+SUM('INPUT - Housing per plan '!T15:T18)</f>
         <v>31177785.086843405</v>
       </c>
@@ -4447,7 +4448,7 @@
       <c r="A26" t="s">
         <v>322</v>
       </c>
-      <c r="B26" s="58">
+      <c r="B26" s="57">
         <f>'INPUT - Housing per plan '!T13+'INPUT - Housing per plan '!T14</f>
         <v>19134889.742555223</v>
       </c>
@@ -4481,7 +4482,7 @@
       <c r="A28" t="s">
         <v>324</v>
       </c>
-      <c r="B28" s="58">
+      <c r="B28" s="57">
         <f>'INPUT - Housing per plan '!T3+SUM('INPUT - Housing per plan '!T19:T21)</f>
         <v>10208915.358117528</v>
       </c>
@@ -4498,7 +4499,7 @@
       <c r="A29" t="s">
         <v>325</v>
       </c>
-      <c r="B29" s="58">
+      <c r="B29" s="57">
         <f>'INPUT - Housing per plan '!T9+'INPUT - Housing per plan '!T10</f>
         <v>2895644.6780366879</v>
       </c>
@@ -4557,7 +4558,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4666,15 +4667,15 @@
       <c r="A11" t="s">
         <v>321</v>
       </c>
-      <c r="B11" s="67">
+      <c r="B11" s="87">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p1",'BASIS - Accessiblity of plans'!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p1"))*100</f>
         <v>72.543445959041293</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="57">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p1",'INPUT - Housing per plan '!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p1"))*100</f>
         <v>100</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="57">
         <f>(SUMIFS('INPUT - Housing per plan '!$O$3:$O$21,'INPUT - Housing per plan '!$E$3:$E$21,"p1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p1"))*100</f>
         <v>0</v>
       </c>
@@ -4683,15 +4684,15 @@
       <c r="A12" t="s">
         <v>322</v>
       </c>
-      <c r="B12" s="67">
+      <c r="B12" s="87">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p2",'BASIS - Accessiblity of plans'!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p2"))*100</f>
         <v>63.157894736842103</v>
       </c>
-      <c r="D12" s="58">
+      <c r="D12" s="57">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p2",'INPUT - Housing per plan '!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p2"))*100</f>
         <v>100</v>
       </c>
-      <c r="F12" s="58">
+      <c r="F12" s="57">
         <f>(SUMIFS('INPUT - Housing per plan '!$O$3:$O$21,'INPUT - Housing per plan '!$E$3:$E$21,"p2"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p2"))*100</f>
         <v>0</v>
       </c>
@@ -4700,15 +4701,15 @@
       <c r="A13" t="s">
         <v>323</v>
       </c>
-      <c r="B13" s="67">
+      <c r="B13" s="87">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p3",'BASIS - Accessiblity of plans'!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p3"))*100</f>
         <v>77.715877437325915</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="57">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p3",'INPUT - Housing per plan '!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p3"))*100</f>
         <v>8.3565459610027855</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="57">
         <f>(SUMIFS('INPUT - Housing per plan '!$O$3:$O$21,'INPUT - Housing per plan '!$E$3:$E$21,"p3"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p3"))*100</f>
         <v>0</v>
       </c>
@@ -4717,15 +4718,15 @@
       <c r="A14" t="s">
         <v>324</v>
       </c>
-      <c r="B14" s="67">
+      <c r="B14" s="87">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p4",'BASIS - Accessiblity of plans'!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p4"))*100</f>
         <v>100</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="57">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p4",'INPUT - Housing per plan '!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p4"))*100</f>
         <v>100</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="57">
         <f>(SUMIFS('INPUT - Housing per plan '!$O$3:$O$21,'INPUT - Housing per plan '!$E$3:$E$21,"p4"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p4"))*100</f>
         <v>0</v>
       </c>
@@ -4734,15 +4735,15 @@
       <c r="A15" t="s">
         <v>325</v>
       </c>
-      <c r="B15" s="67">
+      <c r="B15" s="87">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p5",'BASIS - Accessiblity of plans'!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p5"))*100</f>
         <v>0</v>
       </c>
-      <c r="D15" s="58">
+      <c r="D15" s="57">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p5",'INPUT - Housing per plan '!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p5"))*100</f>
         <v>0</v>
       </c>
-      <c r="F15" s="58">
+      <c r="F15" s="57">
         <f>(SUMIFS('INPUT - Housing per plan '!$O$3:$O$21,'INPUT - Housing per plan '!$E$3:$E$21,"p5"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p5"))*100</f>
         <v>0</v>
       </c>
@@ -4751,15 +4752,15 @@
       <c r="A16" t="s">
         <v>326</v>
       </c>
-      <c r="B16" s="67" t="e">
+      <c r="B16" s="66" t="e">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p6",'BASIS - Accessiblity of plans'!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p6"))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D16" s="58" t="e">
+      <c r="D16" s="57" t="e">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p6",'INPUT - Housing per plan '!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p6"))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F16" s="58" t="e">
+      <c r="F16" s="57" t="e">
         <f>(SUMIFS('INPUT - Housing per plan '!$O$3:$O$21,'INPUT - Housing per plan '!$E$3:$E$21,"p6"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p6"))*100</f>
         <v>#DIV/0!</v>
       </c>
@@ -4768,15 +4769,15 @@
       <c r="A17" t="s">
         <v>327</v>
       </c>
-      <c r="B17" s="67" t="e">
+      <c r="B17" s="66" t="e">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p7",'BASIS - Accessiblity of plans'!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p7"))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D17" s="58" t="e">
+      <c r="D17" s="57" t="e">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p7",'INPUT - Housing per plan '!$F$3:$F$21,"1"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p7"))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F17" s="58" t="e">
+      <c r="F17" s="57" t="e">
         <f>(SUMIFS('INPUT - Housing per plan '!$O$3:$O$21,'INPUT - Housing per plan '!$E$3:$E$21,"p7"))/(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$E$3:$E$21,"p7"))*100</f>
         <v>#DIV/0!</v>
       </c>
@@ -4785,15 +4786,15 @@
       <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="67">
+      <c r="B18" s="66">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'BASIS - Accessiblity of plans'!$F$3:$F$21,"1"))/(SUM('INPUT - Housing per plan '!$L$3:$L$21))*100</f>
         <v>70.978663943677105</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="57">
         <f>(SUMIFS('INPUT - Housing per plan '!$L$3:$L$21,'INPUT - Housing per plan '!$F$3:$F$21,"1"))/(SUM('INPUT - Housing per plan '!$L$3:$L$21))*100</f>
         <v>81.767614338689739</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="57">
         <f>(SUM('INPUT - Housing per plan '!$O$3:$O$21))/(SUM('INPUT - Housing per plan '!$L$3:$L$21))*100</f>
         <v>0</v>
       </c>
@@ -6863,13 +6864,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="58"/>
+    <col min="1" max="1" width="9.140625" style="57"/>
     <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="57" t="s">
         <v>407</v>
       </c>
       <c r="B1" s="1"/>
@@ -6894,7 +6895,7 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="56" t="s">
         <v>395</v>
       </c>
       <c r="E2" t="s">
@@ -6920,7 +6921,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="57" t="s">
         <v>195</v>
       </c>
       <c r="B3" t="s">
@@ -6929,7 +6930,7 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="59">
+      <c r="D3" s="58">
         <v>13</v>
       </c>
       <c r="E3" t="s">
@@ -6956,7 +6957,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="57" t="s">
         <v>199</v>
       </c>
       <c r="B4" t="s">
@@ -6965,7 +6966,7 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="59">
+      <c r="D4" s="58">
         <v>35</v>
       </c>
       <c r="E4" t="s">
@@ -6992,7 +6993,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="57" t="s">
         <v>200</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -7001,7 +7002,7 @@
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="68">
+      <c r="D5" s="67">
         <v>36</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -7028,7 +7029,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="57" t="s">
         <v>201</v>
       </c>
       <c r="B6" t="s">
@@ -7037,7 +7038,7 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="59">
+      <c r="D6" s="58">
         <v>4</v>
       </c>
       <c r="E6" t="s">
@@ -7064,7 +7065,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="57" t="s">
         <v>202</v>
       </c>
       <c r="B7" t="s">
@@ -7073,7 +7074,7 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="58">
         <v>14</v>
       </c>
       <c r="E7" t="s">
@@ -7100,7 +7101,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="57" t="s">
         <v>203</v>
       </c>
       <c r="B8" t="s">
@@ -7109,7 +7110,7 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="59">
+      <c r="D8" s="58">
         <v>2</v>
       </c>
       <c r="E8" t="s">
@@ -7136,7 +7137,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="57" t="s">
         <v>204</v>
       </c>
       <c r="B9" t="s">
@@ -7145,7 +7146,7 @@
       <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="59">
+      <c r="D9" s="58">
         <v>1001</v>
       </c>
       <c r="E9" t="s">
@@ -7172,7 +7173,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="57" t="s">
         <v>206</v>
       </c>
       <c r="B10" t="s">
@@ -7181,7 +7182,7 @@
       <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="59">
+      <c r="D10" s="58">
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -7208,7 +7209,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="57" t="s">
         <v>207</v>
       </c>
       <c r="B11" t="s">
@@ -7217,7 +7218,7 @@
       <c r="C11" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="59">
+      <c r="D11" s="58">
         <v>1339</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -7244,7 +7245,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="57" t="s">
         <v>208</v>
       </c>
       <c r="B12" t="s">
@@ -7253,7 +7254,7 @@
       <c r="C12" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="59">
+      <c r="D12" s="58">
         <v>788</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -7280,7 +7281,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="57" t="s">
         <v>209</v>
       </c>
       <c r="B13" t="s">
@@ -7289,7 +7290,7 @@
       <c r="C13" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="59">
+      <c r="D13" s="58">
         <v>1337</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -7316,7 +7317,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="57" t="s">
         <v>211</v>
       </c>
       <c r="B14" t="s">
@@ -7325,7 +7326,7 @@
       <c r="C14" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="59">
+      <c r="D14" s="58">
         <v>1336</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -7352,185 +7353,185 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="57" t="s">
         <v>408</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="57" t="s">
         <v>397</v>
       </c>
-      <c r="C15" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="59" t="s">
+      <c r="C15" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="58" t="s">
         <v>398</v>
       </c>
       <c r="E15" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="F15" s="58">
+      <c r="F15" s="57">
         <v>740</v>
       </c>
-      <c r="G15" s="60">
+      <c r="G15" s="59">
         <f t="shared" si="0"/>
         <v>925</v>
       </c>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="57" t="s">
         <v>409</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="57" t="s">
         <v>400</v>
       </c>
-      <c r="C16" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="59" t="s">
+      <c r="C16" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="58" t="s">
         <v>399</v>
       </c>
       <c r="E16" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="F16" s="58">
+      <c r="F16" s="57">
         <v>741</v>
       </c>
-      <c r="G16" s="60">
+      <c r="G16" s="59">
         <f t="shared" si="0"/>
         <v>926.25</v>
       </c>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="57" t="s">
         <v>410</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="C17" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="59" t="s">
+      <c r="C17" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="58" t="s">
         <v>396</v>
       </c>
       <c r="E17" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="57">
         <v>694</v>
       </c>
-      <c r="G17" s="60">
+      <c r="G17" s="59">
         <f t="shared" si="0"/>
         <v>867.5</v>
       </c>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="57" t="s">
         <v>411</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="57" t="s">
         <v>394</v>
       </c>
-      <c r="C18" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="59">
+      <c r="C18" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="58">
         <v>1312</v>
       </c>
       <c r="E18" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="57">
         <v>250</v>
       </c>
-      <c r="G18" s="60">
+      <c r="G18" s="59">
         <f t="shared" si="0"/>
         <v>312.5</v>
       </c>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="58"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="57" t="s">
         <v>412</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="57" t="s">
         <v>403</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="59">
+      <c r="D19" s="58">
         <v>3</v>
       </c>
-      <c r="E19" s="58" t="s">
+      <c r="E19" s="57" t="s">
         <v>225</v>
       </c>
-      <c r="F19" s="58">
+      <c r="F19" s="57">
         <v>800</v>
       </c>
-      <c r="G19" s="60">
+      <c r="G19" s="59">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="57" t="s">
         <v>413</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="57" t="s">
         <v>404</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="59">
+      <c r="D20" s="58">
         <v>5</v>
       </c>
-      <c r="E20" s="58" t="s">
+      <c r="E20" s="57" t="s">
         <v>225</v>
       </c>
-      <c r="F20" s="58">
+      <c r="F20" s="57">
         <v>200</v>
       </c>
-      <c r="G20" s="60">
+      <c r="G20" s="59">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="57" t="s">
         <v>414</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="57" t="s">
         <v>405</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="59">
+      <c r="D21" s="58">
         <v>6</v>
       </c>
-      <c r="E21" s="58" t="s">
+      <c r="E21" s="57" t="s">
         <v>225</v>
       </c>
-      <c r="F21" s="58">
+      <c r="F21" s="57">
         <v>200</v>
       </c>
-      <c r="G21" s="60">
+      <c r="G21" s="59">
         <f>F21*1.25</f>
         <v>250</v>
       </c>
@@ -7542,7 +7543,7 @@
       <c r="G23" s="34"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="57" t="s">
         <v>424</v>
       </c>
       <c r="F24" s="3"/>
@@ -8354,11 +8355,11 @@
         <v>0.13095238095238093</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+    <row r="15" spans="1:17" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="57" t="s">
         <v>397</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="57" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="51" t="s">
@@ -8373,50 +8374,50 @@
       <c r="F15" s="51">
         <v>1</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G15" s="57">
         <v>5500</v>
       </c>
-      <c r="H15" s="58">
+      <c r="H15" s="57">
         <v>8</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="57">
         <f>1/H15</f>
         <v>0.125</v>
       </c>
-      <c r="J15" s="58" t="s">
+      <c r="J15" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="K15" s="58">
+      <c r="K15" s="57">
         <v>600</v>
       </c>
-      <c r="L15" s="58">
+      <c r="L15" s="57">
         <v>7</v>
       </c>
       <c r="M15" s="51">
         <f>1/L15</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="N15" s="58">
+      <c r="N15" s="57">
         <v>3</v>
       </c>
       <c r="O15" s="51">
         <f>1/N15</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="P15" s="58">
+      <c r="P15" s="57">
         <f>O15/2+M15/2</f>
         <v>0.23809523809523808</v>
       </c>
-      <c r="Q15" s="58">
+      <c r="Q15" s="57">
         <f>I15/2+M15/2+O15/2</f>
         <v>0.30059523809523808</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="58" t="s">
+    <row r="16" spans="1:17" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="57" t="s">
         <v>400</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="57" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="51" t="s">
@@ -8431,50 +8432,50 @@
       <c r="F16" s="51">
         <v>1</v>
       </c>
-      <c r="G16" s="58">
+      <c r="G16" s="57">
         <v>4300</v>
       </c>
-      <c r="H16" s="58">
+      <c r="H16" s="57">
         <v>7</v>
       </c>
-      <c r="I16" s="58">
+      <c r="I16" s="57">
         <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="J16" s="58" t="s">
+      <c r="J16" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="K16" s="58">
+      <c r="K16" s="57">
         <v>400</v>
       </c>
-      <c r="L16" s="58">
+      <c r="L16" s="57">
         <v>5</v>
       </c>
       <c r="M16" s="51">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="N16" s="58">
+      <c r="N16" s="57">
         <v>2</v>
       </c>
       <c r="O16" s="51">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="P16" s="58">
+      <c r="P16" s="57">
         <f t="shared" si="3"/>
         <v>0.35</v>
       </c>
-      <c r="Q16" s="58">
+      <c r="Q16" s="57">
         <f t="shared" si="4"/>
         <v>0.42142857142857143</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="58" t="s">
+    <row r="17" spans="1:17" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="57" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="51" t="s">
@@ -8489,50 +8490,50 @@
       <c r="F17" s="51">
         <v>1</v>
       </c>
-      <c r="G17" s="58">
+      <c r="G17" s="57">
         <v>6000</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="57">
         <v>9</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="57">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J17" s="58" t="s">
+      <c r="J17" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="K17" s="58">
+      <c r="K17" s="57">
         <v>900</v>
       </c>
-      <c r="L17" s="58">
+      <c r="L17" s="57">
         <v>7</v>
       </c>
       <c r="M17" s="51">
         <f t="shared" si="1"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="N17" s="58">
+      <c r="N17" s="57">
         <v>4</v>
       </c>
       <c r="O17" s="51">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="P17" s="58">
+      <c r="P17" s="57">
         <f t="shared" si="3"/>
         <v>0.19642857142857142</v>
       </c>
-      <c r="Q17" s="58">
+      <c r="Q17" s="57">
         <f t="shared" si="4"/>
         <v>0.25198412698412698</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+    <row r="18" spans="1:17" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="57" t="s">
         <v>394</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="57" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="51" t="s">
@@ -8547,222 +8548,222 @@
       <c r="F18" s="51">
         <v>1</v>
       </c>
-      <c r="G18" s="58">
+      <c r="G18" s="57">
         <v>5200</v>
       </c>
-      <c r="H18" s="58">
+      <c r="H18" s="57">
         <v>8</v>
       </c>
-      <c r="I18" s="58">
+      <c r="I18" s="57">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="J18" s="58" t="s">
+      <c r="J18" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="K18" s="58">
+      <c r="K18" s="57">
         <v>850</v>
       </c>
-      <c r="L18" s="58">
+      <c r="L18" s="57">
         <v>11</v>
       </c>
       <c r="M18" s="51">
         <f t="shared" si="1"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="N18" s="58">
+      <c r="N18" s="57">
         <v>4</v>
       </c>
       <c r="O18" s="51">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="P18" s="58">
+      <c r="P18" s="57">
         <f t="shared" si="3"/>
         <v>0.17045454545454547</v>
       </c>
-      <c r="Q18" s="58">
+      <c r="Q18" s="57">
         <f t="shared" si="4"/>
         <v>0.23295454545454547</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="58" t="s">
+    <row r="19" spans="1:17" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="57" t="s">
         <v>403</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="57" t="s">
         <v>225</v>
       </c>
-      <c r="D19" s="58">
-        <v>1</v>
-      </c>
-      <c r="E19" s="58" t="s">
+      <c r="D19" s="57">
+        <v>1</v>
+      </c>
+      <c r="E19" s="57" t="s">
         <v>406</v>
       </c>
-      <c r="F19" s="58">
-        <v>1</v>
-      </c>
-      <c r="G19" s="58">
+      <c r="F19" s="57">
+        <v>1</v>
+      </c>
+      <c r="G19" s="57">
         <v>1700</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="57">
         <v>6</v>
       </c>
-      <c r="I19" s="58">
+      <c r="I19" s="57">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="J19" s="58" t="s">
+      <c r="J19" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="K19" s="58">
+      <c r="K19" s="57">
         <v>450</v>
       </c>
-      <c r="L19" s="58">
+      <c r="L19" s="57">
         <v>6</v>
       </c>
-      <c r="M19" s="58">
+      <c r="M19" s="57">
         <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="N19" s="58">
+      <c r="N19" s="57">
         <v>6</v>
       </c>
-      <c r="O19" s="58">
+      <c r="O19" s="57">
         <f t="shared" si="2"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P19" s="58">
+      <c r="P19" s="57">
         <f t="shared" si="3"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="Q19" s="58">
+      <c r="Q19" s="57">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="s">
+    <row r="20" spans="1:17" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
         <v>404</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="57" t="s">
         <v>225</v>
       </c>
-      <c r="D20" s="58">
-        <v>1</v>
-      </c>
-      <c r="E20" s="58" t="s">
+      <c r="D20" s="57">
+        <v>1</v>
+      </c>
+      <c r="E20" s="57" t="s">
         <v>406</v>
       </c>
-      <c r="F20" s="60">
-        <v>1</v>
-      </c>
-      <c r="G20" s="58">
+      <c r="F20" s="59">
+        <v>1</v>
+      </c>
+      <c r="G20" s="57">
         <v>1600</v>
       </c>
-      <c r="H20" s="58">
+      <c r="H20" s="57">
         <v>4</v>
       </c>
-      <c r="I20" s="58">
+      <c r="I20" s="57">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="J20" s="58" t="s">
+      <c r="J20" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="K20" s="58">
+      <c r="K20" s="57">
         <v>50</v>
       </c>
-      <c r="L20" s="58">
-        <v>1</v>
-      </c>
-      <c r="M20" s="58">
+      <c r="L20" s="57">
+        <v>1</v>
+      </c>
+      <c r="M20" s="57">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N20" s="58">
-        <v>1</v>
-      </c>
-      <c r="O20" s="58">
+      <c r="N20" s="57">
+        <v>1</v>
+      </c>
+      <c r="O20" s="57">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="P20" s="58">
+      <c r="P20" s="57">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="Q20" s="58">
+      <c r="Q20" s="57">
         <f t="shared" si="4"/>
         <v>1.125</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
+    <row r="21" spans="1:17" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="57" t="s">
         <v>405</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="57" t="s">
         <v>225</v>
       </c>
-      <c r="D21" s="58">
-        <v>1</v>
-      </c>
-      <c r="E21" s="58" t="s">
+      <c r="D21" s="57">
+        <v>1</v>
+      </c>
+      <c r="E21" s="57" t="s">
         <v>406</v>
       </c>
-      <c r="F21" s="60">
-        <v>1</v>
-      </c>
-      <c r="G21" s="58">
+      <c r="F21" s="59">
+        <v>1</v>
+      </c>
+      <c r="G21" s="57">
         <v>1600</v>
       </c>
-      <c r="H21" s="58">
+      <c r="H21" s="57">
         <v>3</v>
       </c>
-      <c r="I21" s="58">
+      <c r="I21" s="57">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J21" s="58" t="s">
+      <c r="J21" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="K21" s="58">
+      <c r="K21" s="57">
         <v>100</v>
       </c>
-      <c r="L21" s="58">
-        <v>1</v>
-      </c>
-      <c r="M21" s="58">
+      <c r="L21" s="57">
+        <v>1</v>
+      </c>
+      <c r="M21" s="57">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N21" s="58">
-        <v>1</v>
-      </c>
-      <c r="O21" s="58">
+      <c r="N21" s="57">
+        <v>1</v>
+      </c>
+      <c r="O21" s="57">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="P21" s="58">
+      <c r="P21" s="57">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="Q21" s="58">
+      <c r="Q21" s="57">
         <f t="shared" si="4"/>
         <v>1.1666666666666665</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:17" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:17" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:17" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8814,10 +8815,10 @@
       <c r="N1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="77" t="s">
+      <c r="P1" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="78" t="s">
+      <c r="Q1" s="77" t="s">
         <v>34</v>
       </c>
     </row>
@@ -8856,14 +8857,14 @@
       <c r="M2" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="78"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="77"/>
     </row>
     <row r="3" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="79"/>
+      <c r="B3" s="78"/>
       <c r="C3" s="3">
         <v>272107</v>
       </c>
@@ -8908,10 +8909,10 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="76"/>
+      <c r="B4" s="75"/>
       <c r="C4">
         <v>4165</v>
       </c>
@@ -8948,24 +8949,24 @@
       <c r="N4">
         <v>0</v>
       </c>
-      <c r="P4" s="58">
+      <c r="P4" s="57">
         <f>'INPUT - Housing per plan '!I3+SUM('INPUT - Housing per plan '!I19:I21)</f>
         <v>2600</v>
       </c>
-      <c r="Q4" s="58">
+      <c r="Q4" s="57">
         <f>C4-P4</f>
         <v>1565</v>
       </c>
-      <c r="R4" s="67">
+      <c r="R4" s="66">
         <f t="shared" ref="R4:R7" si="0">P4/(P4+Q4)</f>
         <v>0.62424969987995194</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="76"/>
+      <c r="B5" s="75"/>
       <c r="C5">
         <v>10014</v>
       </c>
@@ -9016,10 +9017,10 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="76"/>
+      <c r="B6" s="75"/>
       <c r="C6">
         <v>1982</v>
       </c>
@@ -9070,10 +9071,10 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="76"/>
+      <c r="A7" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="75"/>
       <c r="C7">
         <v>23728</v>
       </c>
@@ -9110,15 +9111,15 @@
       <c r="N7">
         <v>10</v>
       </c>
-      <c r="P7" s="58">
+      <c r="P7" s="57">
         <f>SUM('INPUT - Housing per plan '!I11:I18)</f>
         <v>15925</v>
       </c>
-      <c r="Q7" s="58">
+      <c r="Q7" s="57">
         <f>C7-P7</f>
         <v>7803</v>
       </c>
-      <c r="R7" s="67">
+      <c r="R7" s="66">
         <f t="shared" si="0"/>
         <v>0.67114801078894137</v>
       </c>
@@ -9127,15 +9128,15 @@
       <c r="O8" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="58">
+      <c r="P8" s="57">
         <f>SUM(P3:P7)</f>
         <v>23438</v>
       </c>
-      <c r="Q8" s="58">
+      <c r="Q8" s="57">
         <f>SUM(Q3:Q7)</f>
         <v>16451</v>
       </c>
-      <c r="R8" s="67">
+      <c r="R8" s="66">
         <f>P8/(P8+Q8)</f>
         <v>0.58758053598736493</v>
       </c>
@@ -10458,16 +10459,16 @@
       <c r="AB14"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="57" t="s">
         <v>408</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="57" t="s">
         <v>397</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="57" t="s">
         <v>415</v>
       </c>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="57" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="51" t="s">
@@ -10476,40 +10477,40 @@
       <c r="F15" s="51">
         <v>1</v>
       </c>
-      <c r="G15" s="64">
+      <c r="G15" s="63">
         <f>'BASIS - Accessiblity of plans'!P15</f>
         <v>0.23809523809523808</v>
       </c>
-      <c r="H15" s="64">
+      <c r="H15" s="63">
         <f>'BASIS - Accessiblity of plans'!I15</f>
         <v>0.125</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="57">
         <v>740</v>
       </c>
-      <c r="J15" s="60">
+      <c r="J15" s="59">
         <f>I15*1.25</f>
         <v>925</v>
       </c>
-      <c r="K15" s="66">
+      <c r="K15" s="65">
         <v>90</v>
       </c>
-      <c r="L15" s="66">
+      <c r="L15" s="65">
         <f>K15/100*J15</f>
         <v>832.5</v>
       </c>
-      <c r="M15" s="66">
-        <v>0</v>
-      </c>
-      <c r="N15" s="58">
+      <c r="M15" s="65">
+        <v>0</v>
+      </c>
+      <c r="N15" s="57">
         <f>L15*(100-M15)/100</f>
         <v>832.5</v>
       </c>
-      <c r="O15" s="58">
+      <c r="O15" s="57">
         <f>L15*M15/100</f>
         <v>0</v>
       </c>
-      <c r="P15" s="58" t="str">
+      <c r="P15" s="57" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
@@ -10525,7 +10526,7 @@
         <f>IF($F15=1,$O15*('BASIS - Financial data'!$H11-'BASIS - Financial data'!$D11)*(1+Q15),$O15*('BASIS - Financial data'!$I11-'BASIS - Financial data'!$F11))*(1+Q15)</f>
         <v>0</v>
       </c>
-      <c r="T15" s="58">
+      <c r="T15" s="57">
         <f t="shared" si="5"/>
         <v>6707282.4044956733</v>
       </c>
@@ -10535,16 +10536,16 @@
       <c r="AB15"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="57" t="s">
         <v>409</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="57" t="s">
         <v>400</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="57" t="s">
         <v>393</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="57" t="s">
         <v>1</v>
       </c>
       <c r="E16" s="51" t="s">
@@ -10553,40 +10554,40 @@
       <c r="F16" s="51">
         <v>1</v>
       </c>
-      <c r="G16" s="64">
+      <c r="G16" s="63">
         <f>'BASIS - Accessiblity of plans'!P16</f>
         <v>0.35</v>
       </c>
-      <c r="H16" s="64">
+      <c r="H16" s="63">
         <f>'BASIS - Accessiblity of plans'!I16</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="I16" s="58">
+      <c r="I16" s="57">
         <v>741</v>
       </c>
-      <c r="J16" s="60">
+      <c r="J16" s="59">
         <f t="shared" si="1"/>
         <v>926.25</v>
       </c>
-      <c r="K16" s="66">
+      <c r="K16" s="65">
         <v>100</v>
       </c>
-      <c r="L16" s="66">
+      <c r="L16" s="65">
         <f t="shared" si="2"/>
         <v>926.25</v>
       </c>
-      <c r="M16" s="66">
-        <v>0</v>
-      </c>
-      <c r="N16" s="58">
+      <c r="M16" s="65">
+        <v>0</v>
+      </c>
+      <c r="N16" s="57">
         <f t="shared" si="3"/>
         <v>926.25</v>
       </c>
-      <c r="O16" s="58">
+      <c r="O16" s="57">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P16" s="58" t="str">
+      <c r="P16" s="57" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
@@ -10602,7 +10603,7 @@
         <f>IF($F16=1,$O16*('BASIS - Financial data'!$H11-'BASIS - Financial data'!$D11)*(1+Q16),$O16*('BASIS - Financial data'!$I11-'BASIS - Financial data'!$F11))*(1+Q16)</f>
         <v>0</v>
       </c>
-      <c r="T16" s="58">
+      <c r="T16" s="57">
         <f t="shared" si="5"/>
         <v>7462606.999596538</v>
       </c>
@@ -10611,13 +10612,13 @@
       <c r="A17" s="51" t="s">
         <v>410</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="57" t="s">
         <v>416</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="57" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="51" t="s">
@@ -10626,40 +10627,40 @@
       <c r="F17" s="51">
         <v>1</v>
       </c>
-      <c r="G17" s="64">
+      <c r="G17" s="63">
         <f>'BASIS - Accessiblity of plans'!P17</f>
         <v>0.19642857142857142</v>
       </c>
-      <c r="H17" s="64">
+      <c r="H17" s="63">
         <f>'BASIS - Accessiblity of plans'!I17</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="57">
         <v>694</v>
       </c>
-      <c r="J17" s="65">
+      <c r="J17" s="64">
         <f>I17*1.25</f>
         <v>867.5</v>
       </c>
-      <c r="K17" s="66">
+      <c r="K17" s="65">
         <v>20</v>
       </c>
-      <c r="L17" s="66">
+      <c r="L17" s="65">
         <f t="shared" si="2"/>
         <v>173.5</v>
       </c>
-      <c r="M17" s="66">
-        <v>0</v>
-      </c>
-      <c r="N17" s="58">
+      <c r="M17" s="65">
+        <v>0</v>
+      </c>
+      <c r="N17" s="57">
         <f t="shared" si="3"/>
         <v>173.5</v>
       </c>
-      <c r="O17" s="58">
+      <c r="O17" s="57">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P17" s="58" t="str">
+      <c r="P17" s="57" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
@@ -10667,7 +10668,7 @@
         <f>SUM('INPUT - Infra Projects'!AR3:AR38)</f>
         <v>0</v>
       </c>
-      <c r="R17" s="58">
+      <c r="R17" s="57">
         <f>IF(F17=1,N17*('BASIS - Financial data'!E11-'BASIS - Financial data'!D11)*(1+Q17),N17*('BASIS - Financial data'!G11-'BASIS - Financial data'!F11))*(1+Q17)</f>
         <v>1397854.0506666659</v>
       </c>
@@ -10675,7 +10676,7 @@
         <f>IF($F17=1,$O17*('BASIS - Financial data'!$H11-'BASIS - Financial data'!$D11)*(1+Q17),$O17*('BASIS - Financial data'!$I11-'BASIS - Financial data'!$F11))*(1+Q17)</f>
         <v>0</v>
       </c>
-      <c r="T17" s="58">
+      <c r="T17" s="57">
         <f t="shared" si="5"/>
         <v>1397854.0506666659</v>
       </c>
@@ -10685,16 +10686,16 @@
       <c r="AB17"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="57" t="s">
         <v>411</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="57" t="s">
         <v>394</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="57" t="s">
         <v>394</v>
       </c>
-      <c r="D18" s="58" t="s">
+      <c r="D18" s="57" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="51" t="s">
@@ -10703,40 +10704,40 @@
       <c r="F18" s="51">
         <v>1</v>
       </c>
-      <c r="G18" s="64">
+      <c r="G18" s="63">
         <f>'BASIS - Accessiblity of plans'!P18</f>
         <v>0.17045454545454547</v>
       </c>
-      <c r="H18" s="64">
+      <c r="H18" s="63">
         <f>'BASIS - Accessiblity of plans'!I18</f>
         <v>0.125</v>
       </c>
-      <c r="I18" s="58">
+      <c r="I18" s="57">
         <v>250</v>
       </c>
-      <c r="J18" s="60">
+      <c r="J18" s="59">
         <f t="shared" si="1"/>
         <v>312.5</v>
       </c>
-      <c r="K18" s="66">
+      <c r="K18" s="65">
         <v>40</v>
       </c>
-      <c r="L18" s="66">
+      <c r="L18" s="65">
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
-      <c r="M18" s="66">
-        <v>0</v>
-      </c>
-      <c r="N18" s="58">
+      <c r="M18" s="65">
+        <v>0</v>
+      </c>
+      <c r="N18" s="57">
         <f t="shared" si="3"/>
         <v>125</v>
       </c>
-      <c r="O18" s="58">
+      <c r="O18" s="57">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P18" s="58" t="str">
+      <c r="P18" s="57" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
@@ -10752,7 +10753,7 @@
         <f>IF($F18=1,$O18*('BASIS - Financial data'!$H11-'BASIS - Financial data'!$D11)*(1+Q18),$O18*('BASIS - Financial data'!$I11-'BASIS - Financial data'!$F11))*(1+Q18)</f>
         <v>0</v>
       </c>
-      <c r="T18" s="58">
+      <c r="T18" s="57">
         <f t="shared" si="5"/>
         <v>1007099.4601344855</v>
       </c>
@@ -10762,58 +10763,58 @@
       <c r="AB18"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="57" t="s">
         <v>412</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="57" t="s">
         <v>403</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="57" t="s">
         <v>403</v>
       </c>
-      <c r="D19" s="58" t="s">
+      <c r="D19" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="58" t="s">
+      <c r="E19" s="57" t="s">
         <v>225</v>
       </c>
       <c r="F19" s="51">
         <v>1</v>
       </c>
-      <c r="G19" s="64">
+      <c r="G19" s="63">
         <f>'BASIS - Accessiblity of plans'!P19</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="H19" s="64">
+      <c r="H19" s="63">
         <f>'BASIS - Accessiblity of plans'!I19</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="I19" s="58">
+      <c r="I19" s="57">
         <v>800</v>
       </c>
-      <c r="J19" s="60">
+      <c r="J19" s="59">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="K19" s="66">
+      <c r="K19" s="65">
         <v>50</v>
       </c>
-      <c r="L19" s="66">
+      <c r="L19" s="65">
         <f t="shared" si="2"/>
         <v>500</v>
       </c>
-      <c r="M19" s="66">
-        <v>0</v>
-      </c>
-      <c r="N19" s="58">
+      <c r="M19" s="65">
+        <v>0</v>
+      </c>
+      <c r="N19" s="57">
         <f t="shared" si="3"/>
         <v>500</v>
       </c>
-      <c r="O19" s="58">
+      <c r="O19" s="57">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P19" s="58" t="str">
+      <c r="P19" s="57" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
@@ -10839,58 +10840,58 @@
       <c r="AB19"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="57" t="s">
         <v>413</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="57" t="s">
         <v>404</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="57" t="s">
         <v>404</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="58" t="s">
+      <c r="E20" s="57" t="s">
         <v>225</v>
       </c>
       <c r="F20" s="51">
         <v>1</v>
       </c>
-      <c r="G20" s="64">
+      <c r="G20" s="63">
         <f>'BASIS - Accessiblity of plans'!P20</f>
         <v>1</v>
       </c>
-      <c r="H20" s="64">
+      <c r="H20" s="63">
         <f>'BASIS - Accessiblity of plans'!I20</f>
         <v>0.25</v>
       </c>
-      <c r="I20" s="58">
+      <c r="I20" s="57">
         <v>200</v>
       </c>
-      <c r="J20" s="60">
+      <c r="J20" s="59">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="K20" s="66">
+      <c r="K20" s="65">
         <v>40</v>
       </c>
-      <c r="L20" s="66">
+      <c r="L20" s="65">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="M20" s="66">
-        <v>0</v>
-      </c>
-      <c r="N20" s="58">
+      <c r="M20" s="65">
+        <v>0</v>
+      </c>
+      <c r="N20" s="57">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="O20" s="58">
+      <c r="O20" s="57">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P20" s="58" t="str">
+      <c r="P20" s="57" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
@@ -10913,58 +10914,58 @@
       <c r="AB20"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="57" t="s">
         <v>414</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="57" t="s">
         <v>405</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="57" t="s">
         <v>405</v>
       </c>
-      <c r="D21" s="58" t="s">
+      <c r="D21" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="58" t="s">
+      <c r="E21" s="57" t="s">
         <v>225</v>
       </c>
       <c r="F21" s="51">
         <v>1</v>
       </c>
-      <c r="G21" s="64">
+      <c r="G21" s="63">
         <f>'BASIS - Accessiblity of plans'!P21</f>
         <v>1</v>
       </c>
-      <c r="H21" s="64">
+      <c r="H21" s="63">
         <f>'BASIS - Accessiblity of plans'!I21</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I21" s="58">
+      <c r="I21" s="57">
         <v>200</v>
       </c>
-      <c r="J21" s="60">
+      <c r="J21" s="59">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="K21" s="66">
+      <c r="K21" s="65">
         <v>50</v>
       </c>
-      <c r="L21" s="66">
+      <c r="L21" s="65">
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
-      <c r="M21" s="66">
-        <v>0</v>
-      </c>
-      <c r="N21" s="58">
+      <c r="M21" s="65">
+        <v>0</v>
+      </c>
+      <c r="N21" s="57">
         <f t="shared" si="3"/>
         <v>125</v>
       </c>
-      <c r="O21" s="58">
+      <c r="O21" s="57">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P21" s="58" t="str">
+      <c r="P21" s="57" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
@@ -11111,7 +11112,7 @@
   </sheetPr>
   <dimension ref="A1:BB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection activeCell="K8" sqref="K8"/>
       <selection pane="topRight" activeCell="X18" sqref="X18"/>
@@ -11121,7 +11122,7 @@
   <cols>
     <col min="2" max="2" width="68" customWidth="1"/>
     <col min="3" max="3" width="38.140625" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="57" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
@@ -11143,23 +11144,23 @@
       <c r="A1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="81" t="s">
+      <c r="B1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="80" t="s">
         <v>344</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="61" t="s">
         <v>402</v>
       </c>
       <c r="E1" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="81" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
       <c r="I1" s="27" t="s">
         <v>176</v>
       </c>
@@ -11185,20 +11186,20 @@
       <c r="W1" s="38"/>
       <c r="X1" s="38"/>
       <c r="Y1" s="38"/>
-      <c r="AB1" s="80" t="s">
+      <c r="AB1" s="79" t="s">
         <v>174</v>
       </c>
-      <c r="AC1" s="80"/>
-      <c r="AD1" s="80"/>
-      <c r="AE1" s="80"/>
-      <c r="AF1" s="80"/>
-      <c r="AG1" s="80" t="s">
+      <c r="AC1" s="79"/>
+      <c r="AD1" s="79"/>
+      <c r="AE1" s="79"/>
+      <c r="AF1" s="79"/>
+      <c r="AG1" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="AH1" s="80"/>
-      <c r="AI1" s="80"/>
-      <c r="AJ1" s="80"/>
-      <c r="AK1" s="80"/>
+      <c r="AH1" s="79"/>
+      <c r="AI1" s="79"/>
+      <c r="AJ1" s="79"/>
+      <c r="AK1" s="79"/>
       <c r="AL1" s="1" t="s">
         <v>307</v>
       </c>
@@ -11213,9 +11214,9 @@
       </c>
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="62"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="61"/>
       <c r="E2" s="30"/>
       <c r="F2" s="26" t="s">
         <v>172</v>
@@ -11238,12 +11239,12 @@
       <c r="L2" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="M2" s="80" t="s">
+      <c r="M2" s="79" t="s">
         <v>228</v>
       </c>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
       <c r="Q2" s="26" t="s">
         <v>229</v>
       </c>
@@ -11724,7 +11725,7 @@
       <c r="H5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="69">
+      <c r="I5" s="68">
         <v>20</v>
       </c>
       <c r="J5" s="24" t="s">
@@ -16752,174 +16753,174 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:54" s="70" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="70">
+    <row r="34" spans="1:54" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="69">
         <v>34</v>
       </c>
-      <c r="B34" s="70" t="s">
+      <c r="B34" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="70" t="s">
+      <c r="C34" s="69" t="s">
         <v>376</v>
       </c>
-      <c r="D34" s="71" t="s">
+      <c r="D34" s="70" t="s">
         <v>455</v>
       </c>
-      <c r="E34" s="70" t="s">
+      <c r="E34" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="F34" s="70" t="s">
+      <c r="F34" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="G34" s="70" t="s">
+      <c r="G34" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="H34" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="I34" s="75">
+      <c r="H34" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" s="74">
         <v>0.5</v>
       </c>
-      <c r="J34" s="72" t="s">
+      <c r="J34" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="K34" s="70" t="s">
+      <c r="K34" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="L34" s="70">
+      <c r="L34" s="69">
         <v>0.5</v>
       </c>
-      <c r="M34" s="73" t="s">
+      <c r="M34" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="Q34" s="73" t="s">
+      <c r="Q34" s="72" t="s">
         <v>227</v>
       </c>
-      <c r="R34" s="70">
-        <v>0</v>
-      </c>
-      <c r="S34" s="74">
-        <v>0</v>
-      </c>
-      <c r="T34" s="74">
-        <v>0</v>
-      </c>
-      <c r="U34" s="74">
-        <v>0</v>
-      </c>
-      <c r="V34" s="74">
-        <v>0</v>
-      </c>
-      <c r="W34" s="74">
-        <v>0</v>
-      </c>
-      <c r="X34" s="74">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="74">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="70" t="str">
+      <c r="R34" s="69">
+        <v>0</v>
+      </c>
+      <c r="S34" s="73">
+        <v>0</v>
+      </c>
+      <c r="T34" s="73">
+        <v>0</v>
+      </c>
+      <c r="U34" s="73">
+        <v>0</v>
+      </c>
+      <c r="V34" s="73">
+        <v>0</v>
+      </c>
+      <c r="W34" s="73">
+        <v>0</v>
+      </c>
+      <c r="X34" s="73">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="73">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="69" t="str">
         <f t="shared" si="0"/>
         <v>FALSE</v>
       </c>
-      <c r="AA34" s="70" t="s">
+      <c r="AA34" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="AB34" s="70">
-        <v>0</v>
-      </c>
-      <c r="AC34" s="70">
-        <v>0</v>
-      </c>
-      <c r="AD34" s="70">
-        <v>0</v>
-      </c>
-      <c r="AE34" s="70">
-        <v>0</v>
-      </c>
-      <c r="AF34" s="70">
-        <v>0</v>
-      </c>
-      <c r="AG34" s="70">
-        <v>0</v>
-      </c>
-      <c r="AH34" s="70">
-        <v>0</v>
-      </c>
-      <c r="AI34" s="70">
-        <v>0</v>
-      </c>
-      <c r="AJ34" s="70">
-        <v>0</v>
-      </c>
-      <c r="AK34" s="70">
-        <v>1</v>
-      </c>
-      <c r="AL34" s="70">
+      <c r="AB34" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="69">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="69">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="69">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="69">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="69">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="69">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="69">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="69">
+        <v>0</v>
+      </c>
+      <c r="AK34" s="69">
+        <v>1</v>
+      </c>
+      <c r="AL34" s="69">
         <v>0.05</v>
       </c>
-      <c r="AM34" s="70">
+      <c r="AM34" s="69">
         <f t="shared" si="1"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="AN34" s="70">
+      <c r="AN34" s="69">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AO34" s="70">
+      <c r="AO34" s="69">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AP34" s="70">
+      <c r="AP34" s="69">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AQ34" s="70">
+      <c r="AQ34" s="69">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AR34" s="70">
+      <c r="AR34" s="69">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AS34" s="70">
+      <c r="AS34" s="69">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AT34" s="70">
+      <c r="AT34" s="69">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AU34" s="70">
+      <c r="AU34" s="69">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AV34" s="70">
+      <c r="AV34" s="69">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AW34" s="70">
+      <c r="AW34" s="69">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AX34" s="70">
+      <c r="AX34" s="69">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AY34" s="70">
+      <c r="AY34" s="69">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AZ34" s="70">
+      <c r="AZ34" s="69">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="BA34" s="70">
+      <c r="BA34" s="69">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="BB34" s="70">
+      <c r="BB34" s="69">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
@@ -16934,7 +16935,7 @@
       <c r="C35" t="s">
         <v>377</v>
       </c>
-      <c r="D35" s="58" t="s">
+      <c r="D35" s="57" t="s">
         <v>450</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -17109,7 +17110,7 @@
       <c r="C36" s="21" t="s">
         <v>378</v>
       </c>
-      <c r="D36" s="63" t="s">
+      <c r="D36" s="62" t="s">
         <v>451</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -17284,7 +17285,7 @@
       <c r="C37" t="s">
         <v>379</v>
       </c>
-      <c r="D37" s="58" t="s">
+      <c r="D37" s="57" t="s">
         <v>452</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -17769,22 +17770,22 @@
       <c r="B1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82" t="s">
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81" t="s">
         <v>222</v>
       </c>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
       <c r="O1" s="35"/>
       <c r="P1" s="35"/>
       <c r="Q1" s="35"/>
@@ -18141,29 +18142,29 @@
       <c r="A10" t="s">
         <v>197</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="82" t="s">
         <v>217</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="82" t="s">
         <v>110</v>
       </c>
       <c r="D10" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="84"/>
-      <c r="C11" s="84"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="83"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
@@ -18192,24 +18193,24 @@
       <c r="Y12" s="3"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="86" t="s">
         <v>385</v>
       </c>
       <c r="B14" t="s">
         <v>391</v>
       </c>
-      <c r="C14" s="85" t="s">
+      <c r="C14" s="84" t="s">
         <v>386</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="85" t="s">
         <v>387</v>
       </c>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="87"/>
-      <c r="C15" s="85"/>
+      <c r="A15" s="86"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="1" t="s">
         <v>388</v>
       </c>
@@ -18253,7 +18254,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="83"/>
       <c r="B18" s="83"/>
-      <c r="D18" s="58" t="s">
+      <c r="D18" s="57" t="s">
         <v>365</v>
       </c>
     </row>
@@ -18330,7 +18331,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="84" t="s">
+      <c r="A27" s="82" t="s">
         <v>198</v>
       </c>
       <c r="B27" s="83" t="s">
@@ -18350,7 +18351,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="84"/>
+      <c r="A28" s="82"/>
       <c r="B28" s="83"/>
       <c r="C28" s="3" t="s">
         <v>22</v>
@@ -18360,7 +18361,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="84"/>
+      <c r="A29" s="82"/>
       <c r="B29" s="83"/>
       <c r="C29" t="s">
         <v>23</v>
@@ -18370,7 +18371,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="84"/>
+      <c r="A30" s="82"/>
       <c r="B30" s="83"/>
       <c r="C30" t="s">
         <v>24</v>
@@ -18380,7 +18381,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="84"/>
+      <c r="A31" s="82"/>
       <c r="B31" s="83"/>
       <c r="C31" t="s">
         <v>25</v>
@@ -18514,6 +18515,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B26"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="H1:N1"/>
     <mergeCell ref="C1:G1"/>
@@ -18522,21 +18538,6 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -18550,8 +18551,8 @@
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18704,18 +18705,18 @@
       <c r="A10" t="s">
         <v>321</v>
       </c>
-      <c r="B10" s="56">
-        <v>0</v>
-      </c>
-      <c r="C10" s="56">
+      <c r="B10" s="20">
+        <v>0</v>
+      </c>
+      <c r="C10" s="20">
         <f>(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!S3:S38,"1",'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p1"))/(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p1"))*100</f>
         <v>0</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="20">
         <f>SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!S3:S38,"1",'INPUT - Infra Projects'!AA3:AA38,"PT",'INPUT - Infra Projects'!M3:M38,"p1")</f>
         <v>0</v>
       </c>
-      <c r="E10" s="56" t="e">
+      <c r="E10" s="20" t="e">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p1"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p1"))*100</f>
         <v>#DIV/0!</v>
       </c>
@@ -18724,18 +18725,18 @@
       <c r="A11" t="s">
         <v>322</v>
       </c>
-      <c r="B11" s="56">
-        <v>0</v>
-      </c>
-      <c r="C11" s="56">
+      <c r="B11" s="20">
+        <v>0</v>
+      </c>
+      <c r="C11" s="20">
         <f>SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!S3:S38,"1",'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p2")/SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p2")*100</f>
         <v>0</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="20">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p2"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p2"))*100</f>
         <v>0</v>
       </c>
-      <c r="E11" s="56" t="e">
+      <c r="E11" s="20" t="e">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p2"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p2"))*100</f>
         <v>#DIV/0!</v>
       </c>
@@ -18744,18 +18745,18 @@
       <c r="A12" t="s">
         <v>323</v>
       </c>
-      <c r="B12" s="56">
-        <v>0</v>
-      </c>
-      <c r="C12" s="56">
+      <c r="B12" s="20">
+        <v>0</v>
+      </c>
+      <c r="C12" s="20">
         <f>SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!S3:S38,"1",'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p3")/SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p3")*100</f>
         <v>0</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="20">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p3"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p3"))*100</f>
         <v>0</v>
       </c>
-      <c r="E12" s="56">
+      <c r="E12" s="20">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p3"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p3"))*100</f>
         <v>0</v>
       </c>
@@ -18764,18 +18765,18 @@
       <c r="A13" t="s">
         <v>324</v>
       </c>
-      <c r="B13" s="56">
-        <v>0</v>
-      </c>
-      <c r="C13" s="56">
+      <c r="B13" s="20">
+        <v>0</v>
+      </c>
+      <c r="C13" s="20">
         <f>(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!S3:S38,"1",'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p4"))/(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p4"))*100</f>
         <v>0</v>
       </c>
-      <c r="D13" s="56">
+      <c r="D13" s="20">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p4"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p4"))*100</f>
         <v>0</v>
       </c>
-      <c r="E13" s="56">
+      <c r="E13" s="20">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p4"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p4"))*100</f>
         <v>0</v>
       </c>
@@ -18784,18 +18785,18 @@
       <c r="A14" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="56">
-        <v>0</v>
-      </c>
-      <c r="C14" s="56">
+      <c r="B14" s="20">
+        <v>0</v>
+      </c>
+      <c r="C14" s="20">
         <f>(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!S3:S38,"1",'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p5"))/(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p5"))*100</f>
         <v>0</v>
       </c>
-      <c r="D14" s="56" t="e">
+      <c r="D14" s="20" t="e">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p5"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p5"))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E14" s="56" t="e">
+      <c r="E14" s="20" t="e">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p5"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p5"))*100</f>
         <v>#DIV/0!</v>
       </c>
@@ -18804,18 +18805,18 @@
       <c r="A15" t="s">
         <v>326</v>
       </c>
-      <c r="B15" s="56">
-        <v>0</v>
-      </c>
-      <c r="C15" s="56" t="e">
+      <c r="B15" s="20">
+        <v>0</v>
+      </c>
+      <c r="C15" s="20" t="e">
         <f>(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!S3:S38,"1",'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p6"))/(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p6"))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D15" s="56" t="e">
+      <c r="D15" s="20" t="e">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p6"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p6"))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E15" s="56" t="e">
+      <c r="E15" s="20" t="e">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p6"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p6"))*100</f>
         <v>#DIV/0!</v>
       </c>
@@ -18824,38 +18825,44 @@
       <c r="A16" t="s">
         <v>327</v>
       </c>
-      <c r="B16" s="56">
-        <v>0</v>
-      </c>
-      <c r="C16" s="56" t="e">
+      <c r="B16" s="20">
+        <v>0</v>
+      </c>
+      <c r="C16" s="20" t="e">
         <f>(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!S3:S38,"1",'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p7"))/(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!M3:M38,"p7"))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D16" s="56" t="e">
+      <c r="D16" s="20" t="e">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p7"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"PT",'INPUT - Infra Projects'!$M$3:$M$38,"p7"))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E16" s="56" t="e">
+      <c r="E16" s="20" t="e">
         <f>(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$S$3:$S$38,"1",'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p7"))/(SUMIFS('INPUT - Infra Projects'!$AM$3:$AM$38,'INPUT - Infra Projects'!$AA$3:$AA$38,"BIC",'INPUT - Infra Projects'!$M$3:$M$38,"p7"))*100</f>
         <v>#DIV/0!</v>
       </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="56">
-        <v>0</v>
-      </c>
-      <c r="C18" s="4">
+      <c r="B18" s="20">
+        <v>0</v>
+      </c>
+      <c r="C18" s="88">
         <f>(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!S3:S38,"1",'INPUT - Infra Projects'!AA3:AA38,"CAR"))/(SUMIF('INPUT - Infra Projects'!AA3:AA38,"CAR",'INPUT - Infra Projects'!AM3:AM38))*100</f>
         <v>0</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="88">
         <f>(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!S3:S38,"1",'INPUT - Infra Projects'!AA3:AA38,"PT"))/(SUMIF('INPUT - Infra Projects'!AA3:AA38,"PT",'INPUT - Infra Projects'!AM3:AM38))*100</f>
         <v>0</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="88">
         <f>(SUMIFS('INPUT - Infra Projects'!AM3:AM38,'INPUT - Infra Projects'!S3:S38,"1",'INPUT - Infra Projects'!AA3:AA38,"BIC"))/(SUMIF('INPUT - Infra Projects'!AA3:AA38,"BIC",'INPUT - Infra Projects'!AM3:AM38))*100</f>
         <v>0</v>
       </c>

</xml_diff>